<commit_message>
large portion of mlm.html completed and new images added for mlm page
</commit_message>
<xml_diff>
--- a/NN_Model/Theory for Recall and Precision.xlsx
+++ b/NN_Model/Theory for Recall and Precision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Brown\Desktop\Team5_FinalProject\NN_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C85D27D-64F8-46EA-90DD-8A9BCE9ED041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF061694-2B68-44C3-BCED-6FBF81167E14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -253,10 +253,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$9:$C$15</c:f>
+              <c:f>Sheet1!$C$9:$C$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>500</c:v>
                 </c:pt>
@@ -264,18 +264,117 @@
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>4000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>8000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="16">
+                  <c:v>8500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10500</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11500</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13500</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14500</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>16000</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="32">
+                  <c:v>16500</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17500</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>18500</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>19500</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>20000</c:v>
                 </c:pt>
               </c:numCache>
@@ -283,10 +382,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$9:$I$15</c:f>
+              <c:f>Sheet1!$I$9:$I$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>0.32203389830508472</c:v>
                 </c:pt>
@@ -294,18 +393,117 @@
                   <c:v>0.48717948717948717</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.58762886597938147</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.65517241379310343</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>0.70370370370370372</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.74025974025974028</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.76878612716763006</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.79166666666666663</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
+                  <c:v>0.81042654028436023</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.82608695652173914</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8393574297188755</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.85074626865671643</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.86062717770034847</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.86928104575163401</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.87692307692307692</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>0.88372093023255816</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="16">
+                  <c:v>0.88980716253443526</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.89528795811518325</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.90024937655860349</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.90476190476190477</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.90888382687927105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.9126637554585153</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.9161425576519916</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.91935483870967738</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.92233009708737868</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.92509363295880154</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.92766726943942135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.93006993006993011</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.93231810490693734</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.93442622950819676</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.93640699523052462</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>0.93827160493827155</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="32">
+                  <c:v>0.94002998500749624</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.94169096209912539</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.94326241134751776</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.94475138121546964</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.94616419919246297</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.94750656167978997</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.94878361075544171</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>0.95</c:v>
                 </c:pt>
               </c:numCache>
@@ -348,10 +546,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$9:$C$15</c:f>
+              <c:f>Sheet1!$C$9:$C$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>500</c:v>
                 </c:pt>
@@ -359,18 +557,117 @@
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>4000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>8000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="16">
+                  <c:v>8500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10500</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11500</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13500</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14500</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15500</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>16000</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="32">
+                  <c:v>16500</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17500</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>18500</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>19500</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>20000</c:v>
                 </c:pt>
               </c:numCache>
@@ -378,10 +675,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$9:$J$15</c:f>
+              <c:f>Sheet1!$J$9:$J$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>0.95</c:v>
                 </c:pt>
@@ -401,6 +698,105 @@
                   <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>0.95</c:v>
                 </c:pt>
               </c:numCache>
@@ -706,12 +1102,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1294,16 +1685,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1071562</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>274637</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1262062</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>249237</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1594,10 +1985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:L15"/>
+  <dimension ref="A4:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1715,6 +2106,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10" s="1">
+        <f>C9+500</f>
         <v>1000</v>
       </c>
       <c r="D10" s="1">
@@ -1755,15 +2147,16 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11" s="1">
-        <v>2000</v>
+        <f t="shared" ref="C11:C31" si="8">C10+500</f>
+        <v>1500</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>1900</v>
+        <v>1425</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="1"/>
-        <v>100.00000000000009</v>
+        <v>75.000000000000071</v>
       </c>
       <c r="F11" s="1">
         <v>20000</v>
@@ -1778,7 +2171,7 @@
       </c>
       <c r="I11" s="3">
         <f t="shared" si="4"/>
-        <v>0.65517241379310343</v>
+        <v>0.58762886597938147</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="5"/>
@@ -1790,20 +2183,21 @@
       </c>
       <c r="L11" s="2">
         <f t="shared" si="7"/>
-        <v>0.77551020408163263</v>
+        <v>0.72611464968152872</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12" s="1">
-        <v>4000</v>
+        <f t="shared" si="8"/>
+        <v>2000</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>3800</v>
+        <v>1900</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="1"/>
-        <v>200.00000000000017</v>
+        <v>100.00000000000009</v>
       </c>
       <c r="F12" s="1">
         <v>20000</v>
@@ -1818,7 +2212,7 @@
       </c>
       <c r="I12" s="3">
         <f t="shared" si="4"/>
-        <v>0.79166666666666663</v>
+        <v>0.65517241379310343</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="5"/>
@@ -1830,20 +2224,21 @@
       </c>
       <c r="L12" s="2">
         <f t="shared" si="7"/>
-        <v>0.86363636363636354</v>
+        <v>0.77551020408163263</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C13" s="1">
-        <v>8000</v>
+        <f t="shared" si="8"/>
+        <v>2500</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>7600</v>
+        <v>2375</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="1"/>
-        <v>400.00000000000034</v>
+        <v>125.00000000000011</v>
       </c>
       <c r="F13" s="1">
         <v>20000</v>
@@ -1858,7 +2253,7 @@
       </c>
       <c r="I13" s="3">
         <f t="shared" si="4"/>
-        <v>0.88372093023255816</v>
+        <v>0.70370370370370372</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="5"/>
@@ -1870,20 +2265,21 @@
       </c>
       <c r="L13" s="2">
         <f t="shared" si="7"/>
-        <v>0.91566265060240959</v>
+        <v>0.8085106382978724</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" s="1">
-        <v>16000</v>
+        <f t="shared" si="8"/>
+        <v>3000</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>15200</v>
+        <v>2850</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="1"/>
-        <v>800.00000000000068</v>
+        <v>150.00000000000014</v>
       </c>
       <c r="F14" s="1">
         <v>20000</v>
@@ -1898,7 +2294,7 @@
       </c>
       <c r="I14" s="3">
         <f t="shared" si="4"/>
-        <v>0.93827160493827155</v>
+        <v>0.74025974025974028</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="5"/>
@@ -1910,20 +2306,21 @@
       </c>
       <c r="L14" s="2">
         <f t="shared" si="7"/>
-        <v>0.94409937888198758</v>
+        <v>0.83211678832116787</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C15" s="1">
-        <v>20000</v>
+        <f t="shared" si="8"/>
+        <v>3500</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>19000</v>
+        <v>3325</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="1"/>
-        <v>1000.0000000000009</v>
+        <v>175.00000000000014</v>
       </c>
       <c r="F15" s="1">
         <v>20000</v>
@@ -1938,7 +2335,7 @@
       </c>
       <c r="I15" s="3">
         <f t="shared" si="4"/>
-        <v>0.95</v>
+        <v>0.76878612716763006</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="5"/>
@@ -1950,7 +2347,1388 @@
       </c>
       <c r="L15" s="2">
         <f t="shared" si="7"/>
+        <v>0.84984025559105436</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C16" s="1">
+        <f t="shared" si="8"/>
+        <v>4000</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" ref="D16:D31" si="9">$B$4*C16</f>
+        <v>3800</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" ref="E16:E31" si="10">C16*(1-$B$4)</f>
+        <v>200.00000000000017</v>
+      </c>
+      <c r="F16" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" ref="G16:G31" si="11">(F16)*$B$5</f>
+        <v>19000</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" ref="H16:H31" si="12">F16-G16</f>
+        <v>1000</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" ref="I16:I31" si="13">D16/(D16+H16)</f>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" ref="J16:J31" si="14">D16/(D16+E16)</f>
+        <v>0.95</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" ref="K16:K31" si="15">(D16+G16)/(C16+F16)</f>
+        <v>0.95</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" ref="L16:L31" si="16">2*(I16*J16)/(I16+J16)</f>
+        <v>0.86363636363636354</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C17" s="1">
+        <f t="shared" si="8"/>
+        <v>4500</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="9"/>
+        <v>4275</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="10"/>
+        <v>225.0000000000002</v>
+      </c>
+      <c r="F17" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="11"/>
+        <v>19000</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="13"/>
+        <v>0.81042654028436023</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="14"/>
+        <v>0.95</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="15"/>
+        <v>0.95</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="16"/>
+        <v>0.8746803069053708</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C18" s="1">
+        <f t="shared" si="8"/>
+        <v>5000</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="9"/>
+        <v>4750</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="10"/>
+        <v>250.00000000000023</v>
+      </c>
+      <c r="F18" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="11"/>
+        <v>19000</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="13"/>
+        <v>0.82608695652173914</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="14"/>
+        <v>0.95</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="15"/>
+        <v>0.95</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="16"/>
+        <v>0.88372093023255827</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C19" s="1">
+        <f t="shared" si="8"/>
+        <v>5500</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="9"/>
+        <v>5225</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="10"/>
+        <v>275.00000000000023</v>
+      </c>
+      <c r="F19" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="11"/>
+        <v>19000</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="13"/>
+        <v>0.8393574297188755</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="14"/>
+        <v>0.95</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="15"/>
+        <v>0.95</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="16"/>
+        <v>0.8912579957356076</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C20" s="1">
+        <f t="shared" si="8"/>
+        <v>6000</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="9"/>
+        <v>5700</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="10"/>
+        <v>300.00000000000028</v>
+      </c>
+      <c r="F20" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="11"/>
+        <v>19000</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" si="13"/>
+        <v>0.85074626865671643</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="14"/>
+        <v>0.95</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" si="15"/>
+        <v>0.95</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" si="16"/>
+        <v>0.89763779527559051</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C21" s="1">
+        <f t="shared" si="8"/>
+        <v>6500</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="9"/>
+        <v>6175</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="10"/>
+        <v>325.00000000000028</v>
+      </c>
+      <c r="F21" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="11"/>
+        <v>19000</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="13"/>
+        <v>0.86062717770034847</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="14"/>
+        <v>0.95</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" si="15"/>
+        <v>0.95</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="16"/>
+        <v>0.90310786106032914</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C22" s="1">
+        <f t="shared" si="8"/>
+        <v>7000</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="9"/>
+        <v>6650</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="10"/>
+        <v>350.00000000000028</v>
+      </c>
+      <c r="F22" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="11"/>
+        <v>19000</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="13"/>
+        <v>0.86928104575163401</v>
+      </c>
+      <c r="J22" s="1">
+        <f t="shared" si="14"/>
+        <v>0.95</v>
+      </c>
+      <c r="K22" s="1">
+        <f t="shared" si="15"/>
+        <v>0.95</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="16"/>
+        <v>0.9078498293515358</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C23" s="1">
+        <f t="shared" si="8"/>
+        <v>7500</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="9"/>
+        <v>7125</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="10"/>
+        <v>375.00000000000034</v>
+      </c>
+      <c r="F23" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="11"/>
+        <v>19000</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="13"/>
+        <v>0.87692307692307692</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="14"/>
+        <v>0.95</v>
+      </c>
+      <c r="K23" s="1">
+        <f t="shared" si="15"/>
+        <v>0.95</v>
+      </c>
+      <c r="L23" s="2">
+        <f t="shared" si="16"/>
+        <v>0.91200000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C24" s="1">
+        <f t="shared" si="8"/>
+        <v>8000</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="9"/>
+        <v>7600</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="10"/>
+        <v>400.00000000000034</v>
+      </c>
+      <c r="F24" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="11"/>
+        <v>19000</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="13"/>
+        <v>0.88372093023255816</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="14"/>
+        <v>0.95</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" si="15"/>
+        <v>0.95</v>
+      </c>
+      <c r="L24" s="2">
+        <f t="shared" si="16"/>
+        <v>0.91566265060240959</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C25" s="1">
+        <f t="shared" si="8"/>
+        <v>8500</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="9"/>
+        <v>8075</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="10"/>
+        <v>425.0000000000004</v>
+      </c>
+      <c r="F25" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="11"/>
+        <v>19000</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="I25" s="3">
+        <f t="shared" si="13"/>
+        <v>0.88980716253443526</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="14"/>
+        <v>0.95</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" si="15"/>
+        <v>0.95</v>
+      </c>
+      <c r="L25" s="2">
+        <f t="shared" si="16"/>
+        <v>0.91891891891891897</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C26" s="1">
+        <f t="shared" si="8"/>
+        <v>9000</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="9"/>
+        <v>8550</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="10"/>
+        <v>450.0000000000004</v>
+      </c>
+      <c r="F26" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="11"/>
+        <v>19000</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" si="13"/>
+        <v>0.89528795811518325</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="14"/>
+        <v>0.95</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" si="15"/>
+        <v>0.95</v>
+      </c>
+      <c r="L26" s="2">
+        <f t="shared" si="16"/>
+        <v>0.92183288409703501</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C27" s="1">
+        <f t="shared" si="8"/>
+        <v>9500</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="9"/>
+        <v>9025</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="10"/>
+        <v>475.0000000000004</v>
+      </c>
+      <c r="F27" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="11"/>
+        <v>19000</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="I27" s="3">
+        <f t="shared" si="13"/>
+        <v>0.90024937655860349</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="14"/>
+        <v>0.95</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" si="15"/>
+        <v>0.95</v>
+      </c>
+      <c r="L27" s="2">
+        <f t="shared" si="16"/>
+        <v>0.92445582586427655</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C28" s="1">
+        <f t="shared" si="8"/>
+        <v>10000</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="9"/>
+        <v>9500</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="10"/>
+        <v>500.00000000000045</v>
+      </c>
+      <c r="F28" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="11"/>
+        <v>19000</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="13"/>
+        <v>0.90476190476190477</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" si="14"/>
+        <v>0.95</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" si="15"/>
+        <v>0.95</v>
+      </c>
+      <c r="L28" s="2">
+        <f t="shared" si="16"/>
+        <v>0.92682926829268286</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C29" s="1">
+        <f t="shared" si="8"/>
+        <v>10500</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="9"/>
+        <v>9975</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="10"/>
+        <v>525.00000000000045</v>
+      </c>
+      <c r="F29" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="11"/>
+        <v>19000</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" si="13"/>
+        <v>0.90888382687927105</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="14"/>
+        <v>0.95</v>
+      </c>
+      <c r="K29" s="1">
+        <f t="shared" si="15"/>
+        <v>0.95</v>
+      </c>
+      <c r="L29" s="2">
+        <f t="shared" si="16"/>
+        <v>0.92898719441210709</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C30" s="1">
+        <f t="shared" si="8"/>
+        <v>11000</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="9"/>
+        <v>10450</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="10"/>
+        <v>550.00000000000045</v>
+      </c>
+      <c r="F30" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="11"/>
+        <v>19000</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="I30" s="3">
+        <f t="shared" si="13"/>
+        <v>0.9126637554585153</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="14"/>
+        <v>0.95</v>
+      </c>
+      <c r="K30" s="1">
+        <f t="shared" si="15"/>
+        <v>0.95</v>
+      </c>
+      <c r="L30" s="2">
+        <f t="shared" si="16"/>
+        <v>0.93095768374164811</v>
+      </c>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C31" s="1">
+        <f t="shared" si="8"/>
+        <v>11500</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="9"/>
+        <v>10925</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="10"/>
+        <v>575.00000000000045</v>
+      </c>
+      <c r="F31" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="11"/>
+        <v>19000</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="I31" s="3">
+        <f t="shared" si="13"/>
+        <v>0.9161425576519916</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" si="14"/>
+        <v>0.95</v>
+      </c>
+      <c r="K31" s="1">
+        <f t="shared" si="15"/>
+        <v>0.95</v>
+      </c>
+      <c r="L31" s="2">
+        <f t="shared" si="16"/>
+        <v>0.93276414087513326</v>
+      </c>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C32" s="1">
+        <f t="shared" ref="C32:C45" si="17">C31+500</f>
+        <v>12000</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" ref="D32:D45" si="18">$B$4*C32</f>
+        <v>11400</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" ref="E32:E45" si="19">C32*(1-$B$4)</f>
+        <v>600.00000000000057</v>
+      </c>
+      <c r="F32" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" ref="G32:G45" si="20">(F32)*$B$5</f>
+        <v>19000</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" ref="H32:H45" si="21">F32-G32</f>
+        <v>1000</v>
+      </c>
+      <c r="I32" s="3">
+        <f t="shared" ref="I32:I45" si="22">D32/(D32+H32)</f>
+        <v>0.91935483870967738</v>
+      </c>
+      <c r="J32" s="1">
+        <f t="shared" ref="J32:J45" si="23">D32/(D32+E32)</f>
+        <v>0.95</v>
+      </c>
+      <c r="K32" s="1">
+        <f t="shared" ref="K32:K45" si="24">(D32+G32)/(C32+F32)</f>
+        <v>0.95</v>
+      </c>
+      <c r="L32" s="2">
+        <f t="shared" ref="L32:L45" si="25">2*(I32*J32)/(I32+J32)</f>
+        <v>0.93442622950819676</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C33" s="1">
+        <f t="shared" si="17"/>
+        <v>12500</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="18"/>
+        <v>11875</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="19"/>
+        <v>625.00000000000057</v>
+      </c>
+      <c r="F33" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" si="20"/>
+        <v>19000</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="21"/>
+        <v>1000</v>
+      </c>
+      <c r="I33" s="3">
+        <f t="shared" si="22"/>
+        <v>0.92233009708737868</v>
+      </c>
+      <c r="J33" s="1">
+        <f t="shared" si="23"/>
+        <v>0.95</v>
+      </c>
+      <c r="K33" s="1">
+        <f t="shared" si="24"/>
+        <v>0.95</v>
+      </c>
+      <c r="L33" s="2">
+        <f t="shared" si="25"/>
+        <v>0.93596059113300489</v>
+      </c>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C34" s="1">
+        <f t="shared" si="17"/>
+        <v>13000</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="18"/>
+        <v>12350</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="19"/>
+        <v>650.00000000000057</v>
+      </c>
+      <c r="F34" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" si="20"/>
+        <v>19000</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="21"/>
+        <v>1000</v>
+      </c>
+      <c r="I34" s="3">
+        <f t="shared" si="22"/>
+        <v>0.92509363295880154</v>
+      </c>
+      <c r="J34" s="1">
+        <f t="shared" si="23"/>
+        <v>0.95</v>
+      </c>
+      <c r="K34" s="1">
+        <f t="shared" si="24"/>
+        <v>0.95</v>
+      </c>
+      <c r="L34" s="2">
+        <f t="shared" si="25"/>
+        <v>0.93738140417457305</v>
+      </c>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C35" s="1">
+        <f t="shared" si="17"/>
+        <v>13500</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="18"/>
+        <v>12825</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="19"/>
+        <v>675.00000000000057</v>
+      </c>
+      <c r="F35" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G35" s="1">
+        <f t="shared" si="20"/>
+        <v>19000</v>
+      </c>
+      <c r="H35" s="1">
+        <f t="shared" si="21"/>
+        <v>1000</v>
+      </c>
+      <c r="I35" s="3">
+        <f t="shared" si="22"/>
+        <v>0.92766726943942135</v>
+      </c>
+      <c r="J35" s="1">
+        <f t="shared" si="23"/>
+        <v>0.95</v>
+      </c>
+      <c r="K35" s="1">
+        <f t="shared" si="24"/>
+        <v>0.95</v>
+      </c>
+      <c r="L35" s="2">
+        <f t="shared" si="25"/>
+        <v>0.93870082342177497</v>
+      </c>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C36" s="1">
+        <f t="shared" si="17"/>
+        <v>14000</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="18"/>
+        <v>13300</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" si="19"/>
+        <v>700.00000000000057</v>
+      </c>
+      <c r="F36" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G36" s="1">
+        <f t="shared" si="20"/>
+        <v>19000</v>
+      </c>
+      <c r="H36" s="1">
+        <f t="shared" si="21"/>
+        <v>1000</v>
+      </c>
+      <c r="I36" s="3">
+        <f t="shared" si="22"/>
+        <v>0.93006993006993011</v>
+      </c>
+      <c r="J36" s="1">
+        <f t="shared" si="23"/>
+        <v>0.95</v>
+      </c>
+      <c r="K36" s="1">
+        <f t="shared" si="24"/>
+        <v>0.95</v>
+      </c>
+      <c r="L36" s="2">
+        <f t="shared" si="25"/>
+        <v>0.93992932862190814</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C37" s="1">
+        <f t="shared" si="17"/>
+        <v>14500</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="18"/>
+        <v>13775</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="19"/>
+        <v>725.00000000000068</v>
+      </c>
+      <c r="F37" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G37" s="1">
+        <f t="shared" si="20"/>
+        <v>19000</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" si="21"/>
+        <v>1000</v>
+      </c>
+      <c r="I37" s="3">
+        <f t="shared" si="22"/>
+        <v>0.93231810490693734</v>
+      </c>
+      <c r="J37" s="1">
+        <f t="shared" si="23"/>
+        <v>0.95</v>
+      </c>
+      <c r="K37" s="1">
+        <f t="shared" si="24"/>
+        <v>0.95</v>
+      </c>
+      <c r="L37" s="2">
+        <f t="shared" si="25"/>
+        <v>0.94107600341588382</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C38" s="1">
+        <f t="shared" si="17"/>
+        <v>15000</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="18"/>
+        <v>14250</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="19"/>
+        <v>750.00000000000068</v>
+      </c>
+      <c r="F38" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G38" s="1">
+        <f t="shared" si="20"/>
+        <v>19000</v>
+      </c>
+      <c r="H38" s="1">
+        <f t="shared" si="21"/>
+        <v>1000</v>
+      </c>
+      <c r="I38" s="3">
+        <f t="shared" si="22"/>
+        <v>0.93442622950819676</v>
+      </c>
+      <c r="J38" s="1">
+        <f t="shared" si="23"/>
+        <v>0.95</v>
+      </c>
+      <c r="K38" s="1">
+        <f t="shared" si="24"/>
+        <v>0.95</v>
+      </c>
+      <c r="L38" s="2">
+        <f t="shared" si="25"/>
+        <v>0.94214876033057837</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C39" s="1">
+        <f t="shared" si="17"/>
+        <v>15500</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="18"/>
+        <v>14725</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="19"/>
+        <v>775.00000000000068</v>
+      </c>
+      <c r="F39" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G39" s="1">
+        <f t="shared" si="20"/>
+        <v>19000</v>
+      </c>
+      <c r="H39" s="1">
+        <f t="shared" si="21"/>
+        <v>1000</v>
+      </c>
+      <c r="I39" s="3">
+        <f t="shared" si="22"/>
+        <v>0.93640699523052462</v>
+      </c>
+      <c r="J39" s="1">
+        <f t="shared" si="23"/>
+        <v>0.95</v>
+      </c>
+      <c r="K39" s="1">
+        <f t="shared" si="24"/>
+        <v>0.95</v>
+      </c>
+      <c r="L39" s="2">
+        <f t="shared" si="25"/>
+        <v>0.94315452361889507</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C40" s="1">
+        <f t="shared" si="17"/>
+        <v>16000</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="18"/>
+        <v>15200</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="19"/>
+        <v>800.00000000000068</v>
+      </c>
+      <c r="F40" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" si="20"/>
+        <v>19000</v>
+      </c>
+      <c r="H40" s="1">
+        <f t="shared" si="21"/>
+        <v>1000</v>
+      </c>
+      <c r="I40" s="3">
+        <f t="shared" si="22"/>
+        <v>0.93827160493827155</v>
+      </c>
+      <c r="J40" s="1">
+        <f t="shared" si="23"/>
+        <v>0.95</v>
+      </c>
+      <c r="K40" s="1">
+        <f t="shared" si="24"/>
+        <v>0.95</v>
+      </c>
+      <c r="L40" s="2">
+        <f t="shared" si="25"/>
+        <v>0.94409937888198758</v>
+      </c>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C41" s="1">
+        <f t="shared" si="17"/>
+        <v>16500</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="18"/>
+        <v>15675</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="19"/>
+        <v>825.00000000000068</v>
+      </c>
+      <c r="F41" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" si="20"/>
+        <v>19000</v>
+      </c>
+      <c r="H41" s="1">
+        <f t="shared" si="21"/>
+        <v>1000</v>
+      </c>
+      <c r="I41" s="3">
+        <f t="shared" si="22"/>
+        <v>0.94002998500749624</v>
+      </c>
+      <c r="J41" s="1">
+        <f t="shared" si="23"/>
+        <v>0.95</v>
+      </c>
+      <c r="K41" s="1">
+        <f t="shared" si="24"/>
+        <v>0.95</v>
+      </c>
+      <c r="L41" s="2">
+        <f t="shared" si="25"/>
+        <v>0.94498869630746041</v>
+      </c>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C42" s="1">
+        <f t="shared" si="17"/>
+        <v>17000</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="18"/>
+        <v>16150</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="19"/>
+        <v>850.0000000000008</v>
+      </c>
+      <c r="F42" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" si="20"/>
+        <v>19000</v>
+      </c>
+      <c r="H42" s="1">
+        <f t="shared" si="21"/>
+        <v>1000</v>
+      </c>
+      <c r="I42" s="3">
+        <f t="shared" si="22"/>
+        <v>0.94169096209912539</v>
+      </c>
+      <c r="J42" s="1">
+        <f t="shared" si="23"/>
+        <v>0.95</v>
+      </c>
+      <c r="K42" s="1">
+        <f t="shared" si="24"/>
+        <v>0.95</v>
+      </c>
+      <c r="L42" s="2">
+        <f t="shared" si="25"/>
+        <v>0.94582723279648606</v>
+      </c>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C43" s="1">
+        <f t="shared" si="17"/>
+        <v>17500</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" si="18"/>
+        <v>16625</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="19"/>
+        <v>875.0000000000008</v>
+      </c>
+      <c r="F43" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="20"/>
+        <v>19000</v>
+      </c>
+      <c r="H43" s="1">
+        <f t="shared" si="21"/>
+        <v>1000</v>
+      </c>
+      <c r="I43" s="3">
+        <f t="shared" si="22"/>
+        <v>0.94326241134751776</v>
+      </c>
+      <c r="J43" s="1">
+        <f t="shared" si="23"/>
+        <v>0.95</v>
+      </c>
+      <c r="K43" s="1">
+        <f t="shared" si="24"/>
+        <v>0.95</v>
+      </c>
+      <c r="L43" s="2">
+        <f t="shared" si="25"/>
+        <v>0.94661921708185048</v>
+      </c>
+    </row>
+    <row r="44" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C44" s="1">
+        <f t="shared" si="17"/>
+        <v>18000</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" si="18"/>
+        <v>17100</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="19"/>
+        <v>900.0000000000008</v>
+      </c>
+      <c r="F44" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="20"/>
+        <v>19000</v>
+      </c>
+      <c r="H44" s="1">
+        <f t="shared" si="21"/>
+        <v>1000</v>
+      </c>
+      <c r="I44" s="3">
+        <f t="shared" si="22"/>
+        <v>0.94475138121546964</v>
+      </c>
+      <c r="J44" s="1">
+        <f t="shared" si="23"/>
+        <v>0.95</v>
+      </c>
+      <c r="K44" s="1">
+        <f t="shared" si="24"/>
+        <v>0.95</v>
+      </c>
+      <c r="L44" s="2">
+        <f t="shared" si="25"/>
+        <v>0.94736842105263153</v>
+      </c>
+    </row>
+    <row r="45" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C45" s="1">
+        <f t="shared" si="17"/>
+        <v>18500</v>
+      </c>
+      <c r="D45" s="1">
+        <f t="shared" si="18"/>
+        <v>17575</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="19"/>
+        <v>925.0000000000008</v>
+      </c>
+      <c r="F45" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G45" s="1">
+        <f t="shared" si="20"/>
+        <v>19000</v>
+      </c>
+      <c r="H45" s="1">
+        <f t="shared" si="21"/>
+        <v>1000</v>
+      </c>
+      <c r="I45" s="3">
+        <f t="shared" si="22"/>
+        <v>0.94616419919246297</v>
+      </c>
+      <c r="J45" s="1">
+        <f t="shared" si="23"/>
+        <v>0.95</v>
+      </c>
+      <c r="K45" s="1">
+        <f t="shared" si="24"/>
+        <v>0.95</v>
+      </c>
+      <c r="L45" s="2">
+        <f t="shared" si="25"/>
+        <v>0.94807821982467977</v>
+      </c>
+    </row>
+    <row r="46" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C46" s="1">
+        <f t="shared" ref="C46:C50" si="26">C45+500</f>
+        <v>19000</v>
+      </c>
+      <c r="D46" s="1">
+        <f t="shared" ref="D46:D50" si="27">$B$4*C46</f>
+        <v>18050</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" ref="E46:E50" si="28">C46*(1-$B$4)</f>
+        <v>950.0000000000008</v>
+      </c>
+      <c r="F46" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G46" s="1">
+        <f t="shared" ref="G46:G50" si="29">(F46)*$B$5</f>
+        <v>19000</v>
+      </c>
+      <c r="H46" s="1">
+        <f t="shared" ref="H46:H50" si="30">F46-G46</f>
+        <v>1000</v>
+      </c>
+      <c r="I46" s="3">
+        <f t="shared" ref="I46:I50" si="31">D46/(D46+H46)</f>
+        <v>0.94750656167978997</v>
+      </c>
+      <c r="J46" s="1">
+        <f t="shared" ref="J46:J50" si="32">D46/(D46+E46)</f>
+        <v>0.95</v>
+      </c>
+      <c r="K46" s="1">
+        <f t="shared" ref="K46:K50" si="33">(D46+G46)/(C46+F46)</f>
+        <v>0.95</v>
+      </c>
+      <c r="L46" s="2">
+        <f t="shared" ref="L46:L50" si="34">2*(I46*J46)/(I46+J46)</f>
+        <v>0.94875164257555833</v>
+      </c>
+    </row>
+    <row r="47" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C47" s="1">
+        <f t="shared" si="26"/>
+        <v>19500</v>
+      </c>
+      <c r="D47" s="1">
+        <f t="shared" si="27"/>
+        <v>18525</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="28"/>
+        <v>975.00000000000091</v>
+      </c>
+      <c r="F47" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G47" s="1">
+        <f t="shared" si="29"/>
+        <v>19000</v>
+      </c>
+      <c r="H47" s="1">
+        <f t="shared" si="30"/>
+        <v>1000</v>
+      </c>
+      <c r="I47" s="3">
+        <f t="shared" si="31"/>
+        <v>0.94878361075544171</v>
+      </c>
+      <c r="J47" s="1">
+        <f t="shared" si="32"/>
+        <v>0.95</v>
+      </c>
+      <c r="K47" s="1">
+        <f t="shared" si="33"/>
+        <v>0.95</v>
+      </c>
+      <c r="L47" s="2">
+        <f t="shared" si="34"/>
+        <v>0.94939141575912878</v>
+      </c>
+    </row>
+    <row r="48" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C48" s="1">
+        <f t="shared" si="26"/>
+        <v>20000</v>
+      </c>
+      <c r="D48" s="1">
+        <f t="shared" si="27"/>
+        <v>19000</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="28"/>
+        <v>1000.0000000000009</v>
+      </c>
+      <c r="F48" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G48" s="1">
+        <f t="shared" si="29"/>
+        <v>19000</v>
+      </c>
+      <c r="H48" s="1">
+        <f t="shared" si="30"/>
+        <v>1000</v>
+      </c>
+      <c r="I48" s="3">
+        <f t="shared" si="31"/>
+        <v>0.95</v>
+      </c>
+      <c r="J48" s="1">
+        <f t="shared" si="32"/>
+        <v>0.95</v>
+      </c>
+      <c r="K48" s="1">
+        <f t="shared" si="33"/>
+        <v>0.95</v>
+      </c>
+      <c r="L48" s="2">
+        <f t="shared" si="34"/>
         <v>0.95000000000000007</v>
+      </c>
+    </row>
+    <row r="49" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="1"/>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="1"/>
+      <c r="L50" s="2"/>
+    </row>
+    <row r="53" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="F53">
+        <f>25/1025</f>
+        <v>2.4390243902439025E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>